<commit_message>
Lan Atazen Zerrenda eguneratu
</commit_message>
<xml_diff>
--- a/Barne Informazioa/Barne Kudeaketa/Lan Atazen Zerrenda.xlsx
+++ b/Barne Informazioa/Barne Kudeaketa/Lan Atazen Zerrenda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Ingeniaritza Informatikoa\4. Maila\2. Lauhilekoa\GrAL\ProMeta\Barne Informazioa\Barne Kudeaketa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6A87EC41-BA2E-433C-9FCD-428BE95D1858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFC7D88-FC5C-41EE-8F82-6259629A8D9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Lehentasuna</t>
   </si>
@@ -57,9 +57,6 @@
     <t>I1</t>
   </si>
   <si>
-    <t>I4,I5</t>
-  </si>
-  <si>
     <t>I5</t>
   </si>
   <si>
@@ -174,10 +171,10 @@
     <t>I1, I2</t>
   </si>
   <si>
-    <t>I3</t>
-  </si>
-  <si>
     <t>I3,I4</t>
+  </si>
+  <si>
+    <t>I2, I3</t>
   </si>
 </sst>
 </file>
@@ -661,7 +658,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -680,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -692,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
@@ -709,7 +706,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -718,23 +715,23 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -743,23 +740,23 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -768,23 +765,23 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -793,23 +790,23 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -818,23 +815,23 @@
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -843,23 +840,23 @@
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -868,23 +865,23 @@
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -893,23 +890,23 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -918,23 +915,23 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -943,23 +940,23 @@
         <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -968,23 +965,23 @@
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -993,23 +990,23 @@
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1018,23 +1015,23 @@
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1043,23 +1040,23 @@
         <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1068,23 +1065,23 @@
         <v>5</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1093,23 +1090,23 @@
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1118,23 +1115,23 @@
         <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1143,18 +1140,18 @@
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>